<commit_message>
finalizing graphs for report
</commit_message>
<xml_diff>
--- a/jumby_baseline/data/JBB_seagrass.xlsx
+++ b/jumby_baseline/data/JBB_seagrass.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4443" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4449" uniqueCount="177">
   <si>
     <t>date</t>
   </si>
@@ -256,6 +256,9 @@
     <t>donkey dung sea cucumber</t>
   </si>
   <si>
+    <t>cassopea</t>
+  </si>
+  <si>
     <t>Code</t>
   </si>
   <si>
@@ -323,6 +326,9 @@
   </si>
   <si>
     <t>Halophila stipulacea</t>
+  </si>
+  <si>
+    <t>Invasive seagrass</t>
   </si>
   <si>
     <t>HAL</t>
@@ -5479,7 +5485,7 @@
       </c>
       <c r="J2" s="30" t="str">
         <f>VLOOKUP(G2,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="3">
@@ -5683,7 +5689,7 @@
       </c>
       <c r="J8" s="30" t="str">
         <f>VLOOKUP(G8,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="9">
@@ -5853,7 +5859,7 @@
       </c>
       <c r="J13" s="30" t="str">
         <f>VLOOKUP(G13,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="14">
@@ -6023,7 +6029,7 @@
       </c>
       <c r="J18" s="30" t="str">
         <f>VLOOKUP(G18,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="19">
@@ -6193,7 +6199,7 @@
       </c>
       <c r="J23" s="30" t="str">
         <f>VLOOKUP(G23,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="24">
@@ -6363,7 +6369,7 @@
       </c>
       <c r="J28" s="30" t="str">
         <f>VLOOKUP(G28,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="29">
@@ -6499,7 +6505,7 @@
       </c>
       <c r="J32" s="30" t="str">
         <f>VLOOKUP(G32,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="33">
@@ -6669,7 +6675,7 @@
       </c>
       <c r="J37" s="30" t="str">
         <f>VLOOKUP(G37,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="38">
@@ -6941,7 +6947,7 @@
       </c>
       <c r="J45" s="30" t="str">
         <f>VLOOKUP(G45,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="46">
@@ -7179,7 +7185,7 @@
       </c>
       <c r="J52" s="30" t="str">
         <f>VLOOKUP(G52,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="53">
@@ -10069,7 +10075,7 @@
       </c>
       <c r="J137" s="30" t="str">
         <f>VLOOKUP(G137,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="138">
@@ -10273,7 +10279,7 @@
       </c>
       <c r="J143" s="30" t="str">
         <f>VLOOKUP(G143,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="144">
@@ -10443,7 +10449,7 @@
       </c>
       <c r="J148" s="30" t="str">
         <f>VLOOKUP(G148,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="149">
@@ -10579,7 +10585,7 @@
       </c>
       <c r="J152" s="30" t="str">
         <f>VLOOKUP(G152,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="153">
@@ -10817,7 +10823,7 @@
       </c>
       <c r="J159" s="30" t="str">
         <f>VLOOKUP(G159,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="160">
@@ -10885,7 +10891,7 @@
       </c>
       <c r="J161" s="30" t="str">
         <f>VLOOKUP(G161,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="162">
@@ -11157,7 +11163,7 @@
       </c>
       <c r="J169" s="30" t="str">
         <f>VLOOKUP(G169,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="170">
@@ -11327,7 +11333,7 @@
       </c>
       <c r="J174" s="30" t="str">
         <f>VLOOKUP(G174,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="175">
@@ -11497,7 +11503,7 @@
       </c>
       <c r="J179" s="30" t="str">
         <f>VLOOKUP(G179,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="180">
@@ -11633,7 +11639,7 @@
       </c>
       <c r="J183" s="30" t="str">
         <f>VLOOKUP(G183,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="184">
@@ -20207,7 +20213,7 @@
       </c>
       <c r="J438" s="30" t="str">
         <f>VLOOKUP(G438,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="439">
@@ -20815,7 +20821,7 @@
       </c>
       <c r="J457" s="30" t="str">
         <f>VLOOKUP(G457,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="458">
@@ -26167,7 +26173,7 @@
       </c>
       <c r="J619" s="30" t="str">
         <f>VLOOKUP(G619,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="620">
@@ -26303,7 +26309,7 @@
       </c>
       <c r="J623" s="30" t="str">
         <f>VLOOKUP(G623,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="624">
@@ -26405,7 +26411,7 @@
       </c>
       <c r="J626" s="30" t="str">
         <f>VLOOKUP(G626,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="627">
@@ -26575,7 +26581,7 @@
       </c>
       <c r="J631" s="30" t="str">
         <f>VLOOKUP(G631,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="632">
@@ -26711,7 +26717,7 @@
       </c>
       <c r="J635" s="30" t="str">
         <f>VLOOKUP(G635,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="636">
@@ -26949,7 +26955,7 @@
       </c>
       <c r="J642" s="30" t="str">
         <f>VLOOKUP(G642,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="643">
@@ -27051,7 +27057,7 @@
       </c>
       <c r="J645" s="30" t="str">
         <f>VLOOKUP(G645,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="646">
@@ -27289,7 +27295,7 @@
       </c>
       <c r="J652" s="30" t="str">
         <f>VLOOKUP(G652,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="653">
@@ -27459,7 +27465,7 @@
       </c>
       <c r="J657" s="30" t="str">
         <f>VLOOKUP(G657,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="658">
@@ -27867,7 +27873,7 @@
       </c>
       <c r="J669" s="30" t="str">
         <f>VLOOKUP(G669,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="670">
@@ -27935,7 +27941,7 @@
       </c>
       <c r="J671" s="30" t="str">
         <f>VLOOKUP(G671,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="672">
@@ -28275,7 +28281,7 @@
       </c>
       <c r="J681" s="30" t="str">
         <f>VLOOKUP(G681,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="682">
@@ -28445,7 +28451,7 @@
       </c>
       <c r="J686" s="30" t="str">
         <f>VLOOKUP(G686,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="687">
@@ -28751,7 +28757,7 @@
       </c>
       <c r="J695" s="30" t="str">
         <f>VLOOKUP(G695,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="696">
@@ -28853,7 +28859,7 @@
       </c>
       <c r="J698" s="30" t="str">
         <f>VLOOKUP(G698,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="699">
@@ -29193,7 +29199,7 @@
       </c>
       <c r="J708" s="30" t="str">
         <f>VLOOKUP(G708,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="709">
@@ -29567,7 +29573,7 @@
       </c>
       <c r="J719" s="30" t="str">
         <f>VLOOKUP(G719,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="720">
@@ -29771,7 +29777,7 @@
       </c>
       <c r="J725" s="30" t="str">
         <f>VLOOKUP(G725,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="726">
@@ -29903,7 +29909,7 @@
       </c>
       <c r="J729" s="30" t="str">
         <f>VLOOKUP(G729,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="730">
@@ -30063,7 +30069,7 @@
       </c>
       <c r="J734" s="30" t="str">
         <f>VLOOKUP(G734,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="735">
@@ -30191,7 +30197,7 @@
       </c>
       <c r="J738" s="30" t="str">
         <f>VLOOKUP(G738,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="739">
@@ -30383,7 +30389,7 @@
       </c>
       <c r="J744" s="30" t="str">
         <f>VLOOKUP(G744,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="745">
@@ -30543,7 +30549,7 @@
       </c>
       <c r="J749" s="30" t="str">
         <f>VLOOKUP(G749,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="750">
@@ -30767,7 +30773,7 @@
       </c>
       <c r="J756" s="30" t="str">
         <f>VLOOKUP(G756,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="757">
@@ -30927,7 +30933,7 @@
       </c>
       <c r="J761" s="30" t="str">
         <f>VLOOKUP(G761,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="762">
@@ -31087,7 +31093,7 @@
       </c>
       <c r="J766" s="30" t="str">
         <f>VLOOKUP(G766,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="767">
@@ -31311,7 +31317,7 @@
       </c>
       <c r="J773" s="30" t="str">
         <f>VLOOKUP(G773,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="774">
@@ -31727,7 +31733,7 @@
       </c>
       <c r="J786" s="30" t="str">
         <f>VLOOKUP(G786,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="787">
@@ -31855,7 +31861,7 @@
       </c>
       <c r="J790" s="30" t="str">
         <f>VLOOKUP(G790,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="791">
@@ -32015,7 +32021,7 @@
       </c>
       <c r="J795" s="30" t="str">
         <f>VLOOKUP(G795,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="796">
@@ -32175,7 +32181,7 @@
       </c>
       <c r="J800" s="30" t="str">
         <f>VLOOKUP(G800,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="801">
@@ -32335,7 +32341,7 @@
       </c>
       <c r="J805" s="30" t="str">
         <f>VLOOKUP(G805,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="806">
@@ -32495,7 +32501,7 @@
       </c>
       <c r="J810" s="30" t="str">
         <f>VLOOKUP(G810,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="811">
@@ -32655,7 +32661,7 @@
       </c>
       <c r="J815" s="30" t="str">
         <f>VLOOKUP(G815,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="816">
@@ -32847,7 +32853,7 @@
       </c>
       <c r="J821" s="30" t="str">
         <f>VLOOKUP(G821,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="822">
@@ -33039,7 +33045,7 @@
       </c>
       <c r="J827" s="30" t="str">
         <f>VLOOKUP(G827,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="828">
@@ -33231,7 +33237,7 @@
       </c>
       <c r="J833" s="30" t="str">
         <f>VLOOKUP(G833,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="834">
@@ -33527,7 +33533,7 @@
       </c>
       <c r="J842" s="30" t="str">
         <f>VLOOKUP(G842,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="843">
@@ -33663,7 +33669,7 @@
       </c>
       <c r="J846" s="30" t="str">
         <f>VLOOKUP(G846,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="847">
@@ -33867,7 +33873,7 @@
       </c>
       <c r="J852" s="30" t="str">
         <f>VLOOKUP(G852,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="853">
@@ -34173,7 +34179,7 @@
       </c>
       <c r="J861" s="30" t="str">
         <f>VLOOKUP(G861,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="862">
@@ -34275,7 +34281,7 @@
       </c>
       <c r="J864" s="30" t="str">
         <f>VLOOKUP(G864,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="865">
@@ -34411,7 +34417,7 @@
       </c>
       <c r="J868" s="30" t="str">
         <f>VLOOKUP(G868,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="869">
@@ -35567,7 +35573,7 @@
       </c>
       <c r="J902" s="30" t="str">
         <f>VLOOKUP(G902,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="903">
@@ -36572,7 +36578,7 @@
       </c>
       <c r="J932" s="30" t="str">
         <f>VLOOKUP(G932,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="933">
@@ -36727,7 +36733,7 @@
       </c>
       <c r="J937" s="30" t="str">
         <f>VLOOKUP(G937,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="938">
@@ -36944,7 +36950,7 @@
       </c>
       <c r="J944" s="30" t="str">
         <f>VLOOKUP(G944,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="945">
@@ -37130,7 +37136,7 @@
       </c>
       <c r="J950" s="30" t="str">
         <f>VLOOKUP(G950,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="951">
@@ -37471,7 +37477,7 @@
       </c>
       <c r="J961" s="30" t="str">
         <f>VLOOKUP(G961,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="962">
@@ -37595,7 +37601,7 @@
       </c>
       <c r="J965" s="30" t="str">
         <f>VLOOKUP(G965,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="966">
@@ -37843,7 +37849,7 @@
       </c>
       <c r="J973" s="30" t="str">
         <f>VLOOKUP(G973,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="974">
@@ -38091,7 +38097,7 @@
       </c>
       <c r="J981" s="30" t="str">
         <f>VLOOKUP(G981,lookups!$2:$112,3,FALSE)</f>
-        <v>Seagrass</v>
+        <v>Invasive seagrass</v>
       </c>
     </row>
     <row r="982">
@@ -55580,16 +55586,16 @@
         <v>44711.0</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="24">
-        <v>2.0</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>76</v>
+        <v>3.0</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>67</v>
       </c>
       <c r="F16" s="24"/>
       <c r="G16" s="24">
@@ -55604,13 +55610,13 @@
         <v>37</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="24">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="24">
@@ -55631,7 +55637,7 @@
         <v>1.0</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" s="24"/>
       <c r="G18" s="24">
@@ -55649,14 +55655,56 @@
         <v>28</v>
       </c>
       <c r="D19" s="24">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" s="24"/>
       <c r="G19" s="24">
         <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="26">
+        <v>44711.0</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="24">
+        <v>2.0</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="26">
+        <v>44711.0</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="24">
+        <v>4.0</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24">
+        <v>23.0</v>
       </c>
     </row>
   </sheetData>
@@ -55680,13 +55728,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -55714,475 +55762,475 @@
     </row>
     <row r="2">
       <c r="A2" s="33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>86</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="33" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>95</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="33" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="33" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="33" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B12" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="33" t="s">
         <v>107</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="33" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="33" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="33" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="33" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="33" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="33" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="33" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="33" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="33" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="33" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="33" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="33" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="33" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="33" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="33" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B30" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="33" t="s">
         <v>144</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="33" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="33" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B33" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="33" t="s">
         <v>151</v>
-      </c>
-      <c r="C33" s="33" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="33" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C35" s="33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="33" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="33" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C37" s="33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="33" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="33" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B39" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="33" t="s">
         <v>164</v>
-      </c>
-      <c r="C39" s="33" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="33" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C40" s="33" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="33" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B41" s="33" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C41" s="33" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="33" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C42" s="33" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="33" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B44" s="33" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46">

</xml_diff>

<commit_message>
updating seagrass pie charts for clarity
</commit_message>
<xml_diff>
--- a/jumby_baseline/data/JBB_seagrass.xlsx
+++ b/jumby_baseline/data/JBB_seagrass.xlsx
@@ -448,7 +448,7 @@
     <t>Sponge</t>
   </si>
   <si>
-    <t>Sponges, tunicates &amp; soft coral</t>
+    <t>Sponges, tunicates &amp; corals</t>
   </si>
   <si>
     <t>GOR</t>
@@ -469,9 +469,6 @@
     <t>Porites porites</t>
   </si>
   <si>
-    <t>Stony coral</t>
-  </si>
-  <si>
     <t>PFUR</t>
   </si>
   <si>
@@ -481,7 +478,7 @@
     <t>PAST</t>
   </si>
   <si>
-    <t>Porited astreoides</t>
+    <t>Porites astreoides</t>
   </si>
   <si>
     <t>SRAD</t>
@@ -539,6 +536,9 @@
   </si>
   <si>
     <t>Cladocora arbuscula</t>
+  </si>
+  <si>
+    <t>Stony coral</t>
   </si>
   <si>
     <t>CYAN</t>
@@ -13339,7 +13339,7 @@
       </c>
       <c r="J233" s="30" t="str">
         <f>VLOOKUP(G233,lookups!$2:$112,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="234">
@@ -15039,7 +15039,7 @@
       </c>
       <c r="J283" s="30" t="str">
         <f>VLOOKUP(G283,lookups!$2:$112,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="284">
@@ -38345,7 +38345,7 @@
       </c>
       <c r="J989" s="30" t="str">
         <f>VLOOKUP(G989,lookups!$2:$112,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="990">
@@ -40019,7 +40019,7 @@
       </c>
       <c r="J1043" s="30" t="str">
         <f>VLOOKUP(G1043,lookups!$2:$112,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1044">
@@ -46653,7 +46653,7 @@
       </c>
       <c r="J1257" s="30" t="str">
         <f>VLOOKUP(G1257,lookups!$2:$112,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1258">
@@ -48017,7 +48017,7 @@
       </c>
       <c r="J1301" s="30" t="str">
         <f>VLOOKUP(G1301,lookups!$2:$112,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1302">
@@ -48141,7 +48141,7 @@
       </c>
       <c r="J1305" s="30" t="str">
         <f>VLOOKUP(G1305,lookups!$2:$112,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1306">
@@ -48296,7 +48296,7 @@
       </c>
       <c r="J1310" s="30" t="str">
         <f>VLOOKUP(G1310,lookups!$2:$112,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1311">
@@ -49133,7 +49133,7 @@
       </c>
       <c r="J1337" s="30" t="str">
         <f>VLOOKUP(G1337,lookups!$2:$112,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1338">
@@ -49815,7 +49815,7 @@
       </c>
       <c r="J1359" s="30" t="str">
         <f>VLOOKUP(G1359,lookups!$2:$112,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1360">
@@ -50156,7 +50156,7 @@
       </c>
       <c r="J1370" s="30" t="str">
         <f>VLOOKUP(G1370,lookups!$2:$112,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1371">
@@ -50497,7 +50497,7 @@
       </c>
       <c r="J1381" s="30" t="str">
         <f>VLOOKUP(G1381,lookups!$2:$112,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1382">
@@ -50621,7 +50621,7 @@
       </c>
       <c r="J1385" s="30" t="str">
         <f>VLOOKUP(G1385,lookups!$2:$112,3,FALSE)</f>
-        <v>Stony coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1386">
@@ -50807,7 +50807,7 @@
       </c>
       <c r="J1391" s="30" t="str">
         <f>VLOOKUP(G1391,lookups!$2:$112,3,FALSE)</f>
-        <v>Sponges, tunicates &amp; soft coral</v>
+        <v>Sponges, tunicates &amp; corals</v>
       </c>
     </row>
     <row r="1392">
@@ -56098,128 +56098,128 @@
         <v>150</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B33" s="33" t="s">
-        <v>153</v>
-      </c>
       <c r="C33" s="33" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B34" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B34" s="33" t="s">
-        <v>155</v>
-      </c>
       <c r="C34" s="33" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="33" t="s">
-        <v>157</v>
-      </c>
       <c r="C35" s="33" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="33" t="s">
-        <v>159</v>
-      </c>
       <c r="C36" s="33" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="B37" s="33" t="s">
-        <v>161</v>
-      </c>
       <c r="C37" s="33" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="C38" s="33" t="s">
         <v>163</v>
-      </c>
-      <c r="C38" s="33" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="B39" s="33" t="s">
-        <v>166</v>
-      </c>
       <c r="C39" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="B40" s="33" t="s">
-        <v>168</v>
-      </c>
       <c r="C40" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B41" s="33" t="s">
-        <v>170</v>
-      </c>
       <c r="C41" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="B42" s="33" t="s">
-        <v>172</v>
-      </c>
       <c r="C42" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="C43" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="44">

</xml_diff>